<commit_message>
Updated with new soil layers
</commit_message>
<xml_diff>
--- a/agol_layers_metadata.xlsx
+++ b/agol_layers_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://naturalstate3030-my.sharepoint.com/personal/dhenry_naturalstate_org/Documents/ArcPro projects/agol-data-workflows/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3346E674-F38C-4CEF-B239-8A434C535C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="204" documentId="13_ncr:1_{3346E674-F38C-4CEF-B239-8A434C535C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63162DBC-7A47-4623-B00A-CD2BA8792ADA}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AGOL_properties" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="441">
   <si>
     <t>NDVI</t>
   </si>
@@ -621,9 +621,6 @@
   </si>
   <si>
     <t>Rivers</t>
-  </si>
-  <si>
-    <t>06_local_data_source_to_GDB.py</t>
   </si>
   <si>
     <t>River SNIPPET</t>
@@ -1167,12 +1164,293 @@
   <si>
     <t>https://doi.org/10.5194/essd-2019-252</t>
   </si>
+  <si>
+    <t>Vegetation biomass</t>
+  </si>
+  <si>
+    <t>Aboveground Biomass Density</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/earth-engine/datasets/catalog/LARSE_GEDI_GEDI04_B_002#bands</t>
+  </si>
+  <si>
+    <t>https://daac.ornl.gov/GEDI/guides/GEDI_L4B_Gridded_Biomass.html</t>
+  </si>
+  <si>
+    <t>Dubayah, R.O., J. Armston, S.P. Healey, Z. Yang, P.L. Patterson, S. Saarela, G. Stahl, L. Duncanson, and J.R. Kellner. 2022. GEDI L4B Gridded Aboveground Biomass Density, Version 2. ORNL DAAC, Oak Ridge, Tennessee, USA. https://doi.org/10.3334/ORNLDAAC/2017</t>
+  </si>
+  <si>
+    <t>AGBD SNIPPET</t>
+  </si>
+  <si>
+    <t>Biomass density, vegetation biomass</t>
+  </si>
+  <si>
+    <t>Mg/ha</t>
+  </si>
+  <si>
+    <t>GEDI L4B Gridded Aboveground Biomass Density, Version 2</t>
+  </si>
+  <si>
+    <t>megagrams biomass per ha</t>
+  </si>
+  <si>
+    <t>RS_062</t>
+  </si>
+  <si>
+    <t>19_GEDI_L4B.ipynb</t>
+  </si>
+  <si>
+    <t>GEDI</t>
+  </si>
+  <si>
+    <t>RS_063</t>
+  </si>
+  <si>
+    <t>20_GEDI_L2A_L2B.ipynb</t>
+  </si>
+  <si>
+    <t>Canopy metrics</t>
+  </si>
+  <si>
+    <t>GEDI L2A Raster Canopy Top Height (Version 2)</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/earth-engine/datasets/catalog/LARSE_GEDI_GEDI02_A_002_MONTHLY#bands</t>
+  </si>
+  <si>
+    <t>https://lpdaac.usgs.gov/documents/998/GEDI02_UserGuide_V21.pdf</t>
+  </si>
+  <si>
+    <t>Dubayah, R., Hofton, M., J. B. Blair, Armston, J., Tang, H., Luthcke, S. (2021). GEDI L2A Elevation and Height Metrics Data Global Footprint Level V002 [Data set]. NASA EOSDIS Land Processes DAAC. Accessed YYYY-MMDD from https://doi.org/10.5067/GEDI/GEDI02_A.002.</t>
+  </si>
+  <si>
+    <t>Canopy height</t>
+  </si>
+  <si>
+    <t>GEDI L2B Raster Canopy Cover Vertical Profile Metrics (Version 2)</t>
+  </si>
+  <si>
+    <t>RS_064</t>
+  </si>
+  <si>
+    <t>RS_065</t>
+  </si>
+  <si>
+    <t>RS_066</t>
+  </si>
+  <si>
+    <t>Total canopy cover</t>
+  </si>
+  <si>
+    <t>Total plant area index</t>
+  </si>
+  <si>
+    <t>m^2/m^3</t>
+  </si>
+  <si>
+    <t>1 (area fraction)</t>
+  </si>
+  <si>
+    <t>Plant area volume density</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/earth-engine/datasets/catalog/LARSE_GEDI_GEDI02_B_002_MONTHLY#bands</t>
+  </si>
+  <si>
+    <t>https://lpdaac.usgs.gov/documents/588/GEDI_FCCVPM_ATBD_v1.0.pdf</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dubayah, R., Tang, H., Armston, J., Luthcke, S., Hofton, M., Blair, J. (2021). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GEDI L2B Canopy Cover and Vertical Profile Metrics Data Global Footprint Level V002</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [Data set]. NASA EOSDIS Land Processes DAAC. Accessed 2023-06-22 from https://doi.org/10.5067/GEDI/GEDI02_B.002</t>
+    </r>
+  </si>
+  <si>
+    <t>GEDI L2A SNIPPET</t>
+  </si>
+  <si>
+    <t>GEDI L2B SNIPPET</t>
+  </si>
+  <si>
+    <t>Canopy cover</t>
+  </si>
+  <si>
+    <t>Plant area index</t>
+  </si>
+  <si>
+    <t>Plant area volume density profile in 25</t>
+  </si>
+  <si>
+    <t>Mean canopy height (gridded)</t>
+  </si>
+  <si>
+    <t>Canopy top height (lidar footrpint)</t>
+  </si>
+  <si>
+    <t>GEDI L3 Gridded Land Surface Metrics, Version 2</t>
+  </si>
+  <si>
+    <t>RS_067</t>
+  </si>
+  <si>
+    <t>RS_067.py</t>
+  </si>
+  <si>
+    <t>https://daac.ornl.gov/GEDI/guides/GEDI_L3_LandSurface_Metrics_V2.html</t>
+  </si>
+  <si>
+    <t>https://daac.ornl.gov/cgi-bin/dsviewer.pl?ds_id=1952</t>
+  </si>
+  <si>
+    <t>GEDI L3 SNIPPET</t>
+  </si>
+  <si>
+    <t>RS_068</t>
+  </si>
+  <si>
+    <t>RS_068.py</t>
+  </si>
+  <si>
+    <t>Climate</t>
+  </si>
+  <si>
+    <t>Global Aridity Index</t>
+  </si>
+  <si>
+    <t>Global Aridity Index and Potential Evapotranspiration (ET0) Database V3</t>
+  </si>
+  <si>
+    <t>https://figshare.com/articles/dataset/Global_Aridity_Index_and_Potential_Evapotranspiration_ET0_Climate_Database_v2/7504448/6</t>
+  </si>
+  <si>
+    <t>https://figshare.com/articles/dataset/Global_Aridity_Index_and_Potential_Evapotranspiration_ET0_Climate_Database_v2/7504448/6?file=36324084</t>
+  </si>
+  <si>
+    <t>Zomer, R. J., Trabucco, A. 2022. Version 3 of the “Global Aridity Index and Potential
+Evapotranspiration (ET0) Database”: Estimation of Penman-Monteith Reference Evapotranspiration. (In
+Press). Available online from the CGIAR-CSI GeoPortal at: https://cgiarcsi.community/2019/01/24/globalaridity-
+index-and-potential-evapotranspiration-climate-database-v3/</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41597-022-01493-1</t>
+  </si>
+  <si>
+    <t>GAI SNIPPET</t>
+  </si>
+  <si>
+    <t>Climate, Aridity Index</t>
+  </si>
+  <si>
+    <t>RS_069</t>
+  </si>
+  <si>
+    <t>21_iSDAsoil.pynb</t>
+  </si>
+  <si>
+    <t>Effective Cation Exchange Capacity</t>
+  </si>
+  <si>
+    <t>iSDAsoil Effective Cation Exchange Capacity</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/earth-engine/datasets/catalog/ISDASOIL_Africa_v1_cation_exchange_capacity#description</t>
+  </si>
+  <si>
+    <t>Hengl, T., Miller, M.A.E., Križan, J., et al. African soil properties and nutrients mapped at 30 m spatial resolution using two-scale ensemble machine learning. Sci Rep 11, 6130 (2021). doi:10.1038/s41598-021-85639-y</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41598-021-85639-y</t>
+  </si>
+  <si>
+    <t>Soil Cation Exchange Capacity SNIPPET</t>
+  </si>
+  <si>
+    <t>Soils, Cation exchange capacity</t>
+  </si>
+  <si>
+    <t>cmol(+)/kg</t>
+  </si>
+  <si>
+    <t>Layer is average of two depth bands (0-20cm and 20-50cm)</t>
+  </si>
+  <si>
+    <t>RS_070</t>
+  </si>
+  <si>
+    <t>22_OLM_Soil_Taxonomy.ipynb</t>
+  </si>
+  <si>
+    <t>Soil Taxonomy</t>
+  </si>
+  <si>
+    <t>OpenLandMap USDA Soil Taxonomy Great Groups</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/earth-engine/datasets/catalog/OpenLandMap_SOL_SOL_GRTGROUP_USDA-SOILTAX_C_v01#description</t>
+  </si>
+  <si>
+    <t>Tomislav Hengl, &amp; Travis Nauman. (2018). Predicted USDA soil great groups at 250 m (probabilities) (Version v01) [Data set]. Zenodo. 10.5281/zenodo.1476844</t>
+  </si>
+  <si>
+    <t>https://www.nrcs.usda.gov/sites/default/files/2022-06/Illustrated_Guide_to_Soil_Taxonomy.pdf</t>
+  </si>
+  <si>
+    <t>See band description in GEE page for vpixel value key</t>
+  </si>
+  <si>
+    <t>Soil Taxonomy SNIPPET</t>
+  </si>
+  <si>
+    <t>Soils, Soil Taxonmy</t>
+  </si>
+  <si>
+    <t>RS_071</t>
+  </si>
+  <si>
+    <t>RS_071.py</t>
+  </si>
+  <si>
+    <t>https://esdac.jrc.ec.europa.eu/content/soil-map-soil-atlas-africa</t>
+  </si>
+  <si>
+    <t>Dewitte, O., Jones, A., Spaargaren, O., Breuning-Madsen, H., Brossard, M., Dampha, A., Deckers, J., Gallali, T., Hallet, S., Jones, R., Kilasara, M., Le Roux, P., Michéli, E., Montanarella, L., Thiombiano, L., Van Ranst, E., Yemefack, M., Zougmore, R., 2013. Harmonisation of the soil map of Africa at the continental scale. Geoderma, 211-212, 138-153</t>
+  </si>
+  <si>
+    <t>Soil Atlas SNIPPET</t>
+  </si>
+  <si>
+    <t>Soils, Soil Atlas</t>
+  </si>
+  <si>
+    <t>https://esdac.jrc.ec.europa.eu/Library/Maps/Africa_Atlas/Documents/JRC_africa_soil_atlas_part1.pdf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1221,6 +1499,14 @@
       <color rgb="FF222222"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1278,6 +1564,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1543,13 +1833,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC57E1D-8C4C-418F-9437-3E9925023977}">
-  <dimension ref="A1:U62"/>
+  <dimension ref="A1:T72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1571,19 +1861,19 @@
     <col min="16" max="16" width="27.109375" customWidth="1"/>
     <col min="17" max="17" width="10.6640625" style="2" customWidth="1"/>
     <col min="18" max="18" width="33.44140625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="36.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>64</v>
@@ -1619,7 +1909,7 @@
         <v>7</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>8</v>
@@ -1630,14 +1920,14 @@
       <c r="R1" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="S1" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="T1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="U1" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
@@ -1645,7 +1935,7 @@
         <v>130</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
@@ -1660,7 +1950,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I2" s="2">
         <v>30</v>
@@ -1675,7 +1965,7 @@
         <v>2023</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>13</v>
@@ -1688,16 +1978,16 @@
         <v>0</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1705,7 +1995,7 @@
         <v>131</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
@@ -1750,14 +2040,14 @@
         <f t="shared" ref="R3" si="0">CONCATENATE(O3, " SNIPPET")</f>
         <v xml:space="preserve"> SNIPPET</v>
       </c>
+      <c r="S3" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="T3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1765,7 +2055,7 @@
         <v>131</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>19</v>
@@ -1810,14 +2100,14 @@
         <f>CONCATENATE(O4, " SNIPPET")</f>
         <v xml:space="preserve"> SNIPPET</v>
       </c>
+      <c r="S4" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="T4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1825,7 +2115,7 @@
         <v>132</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>3</v>
@@ -1870,14 +2160,14 @@
         <f t="shared" ref="R5:R12" si="1">CONCATENATE(O5, " SNIPPET")</f>
         <v xml:space="preserve"> SNIPPET</v>
       </c>
+      <c r="S5" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="T5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="U5" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1885,7 +2175,7 @@
         <v>133</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>32</v>
@@ -1927,14 +2217,14 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> SNIPPET</v>
       </c>
+      <c r="S6" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="T6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="U6" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1942,7 +2232,7 @@
         <v>133</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>32</v>
@@ -1987,14 +2277,14 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> SNIPPET</v>
       </c>
+      <c r="S7" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="T7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="U7" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -2002,7 +2292,7 @@
         <v>133</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>32</v>
@@ -2047,22 +2337,22 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> SNIPPET</v>
       </c>
+      <c r="S8" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="T8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="U8" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>32</v>
@@ -2104,22 +2394,22 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> SNIPPET</v>
       </c>
+      <c r="S9" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="T9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>32</v>
@@ -2161,22 +2451,22 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> SNIPPET</v>
       </c>
+      <c r="S10" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="T10" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>32</v>
@@ -2218,22 +2508,22 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> SNIPPET</v>
       </c>
+      <c r="S11" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="T11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>32</v>
@@ -2275,14 +2565,14 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> SNIPPET</v>
       </c>
+      <c r="S12" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="T12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -2290,7 +2580,7 @@
         <v>134</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>80</v>
@@ -2331,14 +2621,14 @@
       <c r="R13" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="S13" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="T13" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="U13" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -2346,7 +2636,7 @@
         <v>135</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>28</v>
@@ -2387,14 +2677,14 @@
       <c r="R14" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="S14" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="T14" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="U14" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -2402,7 +2692,7 @@
         <v>136</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>102</v>
@@ -2446,14 +2736,14 @@
       <c r="R15" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="S15" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="T15" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="U15" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -2461,7 +2751,7 @@
         <v>136</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>102</v>
@@ -2505,14 +2795,14 @@
       <c r="R16" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="S16" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="T16" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="U16" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -2520,7 +2810,7 @@
         <v>136</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>102</v>
@@ -2564,14 +2854,14 @@
       <c r="R17" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="S17" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="T17" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="U17" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>115</v>
       </c>
@@ -2579,7 +2869,7 @@
         <v>137</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>0</v>
@@ -2625,14 +2915,14 @@
         <f t="shared" ref="R18" si="2">CONCATENATE(O18, " SNIPPET")</f>
         <v xml:space="preserve"> SNIPPET</v>
       </c>
+      <c r="S18" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="T18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U18" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>120</v>
       </c>
@@ -2640,7 +2930,7 @@
         <v>137</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>19</v>
@@ -2686,14 +2976,14 @@
         <f>CONCATENATE(O19, " SNIPPET")</f>
         <v xml:space="preserve"> SNIPPET</v>
       </c>
+      <c r="S19" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="T19" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="U19" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>121</v>
       </c>
@@ -2701,7 +2991,7 @@
         <v>137</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>4</v>
@@ -2746,14 +3036,14 @@
       <c r="R20" s="2" t="s">
         <v>123</v>
       </c>
+      <c r="S20" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="T20" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U20" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -2761,7 +3051,7 @@
         <v>138</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>32</v>
@@ -2802,22 +3092,22 @@
       <c r="R21" s="2" t="s">
         <v>124</v>
       </c>
+      <c r="S21" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="T21" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>139</v>
       </c>
       <c r="B22" t="s">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>140</v>
@@ -2832,7 +3122,7 @@
         <v>191</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>26</v>
@@ -2857,16 +3147,16 @@
         <v>1</v>
       </c>
       <c r="R22" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="S22" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="T22" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="U22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>141</v>
       </c>
@@ -2874,7 +3164,7 @@
         <v>151</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>140</v>
@@ -2915,14 +3205,14 @@
       <c r="R23" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="T23" s="2" t="s">
+      <c r="S23" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="U23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>142</v>
       </c>
@@ -2930,7 +3220,7 @@
         <v>151</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>140</v>
@@ -2971,14 +3261,14 @@
       <c r="R24" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="T24" s="2" t="s">
+      <c r="S24" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="U24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>143</v>
       </c>
@@ -2986,7 +3276,7 @@
         <v>151</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>140</v>
@@ -3027,14 +3317,14 @@
       <c r="R25" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="T25" s="2" t="s">
+      <c r="S25" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="U25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>144</v>
       </c>
@@ -3042,7 +3332,7 @@
         <v>151</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>140</v>
@@ -3083,14 +3373,14 @@
       <c r="R26" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="T26" s="2" t="s">
+      <c r="S26" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="U26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>145</v>
       </c>
@@ -3098,7 +3388,7 @@
         <v>151</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>140</v>
@@ -3139,14 +3429,14 @@
       <c r="R27" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="T27" s="2" t="s">
+      <c r="S27" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="U27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -3154,7 +3444,7 @@
         <v>151</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>140</v>
@@ -3195,14 +3485,14 @@
       <c r="R28" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="T28" s="2" t="s">
+      <c r="S28" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="U28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>147</v>
       </c>
@@ -3210,7 +3500,7 @@
         <v>151</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>140</v>
@@ -3251,14 +3541,14 @@
       <c r="R29" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="T29" s="2" t="s">
+      <c r="S29" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="U29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>148</v>
       </c>
@@ -3266,7 +3556,7 @@
         <v>151</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>140</v>
@@ -3307,14 +3597,14 @@
       <c r="R30" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="T30" s="2" t="s">
+      <c r="S30" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="U30" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>149</v>
       </c>
@@ -3322,7 +3612,7 @@
         <v>151</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>140</v>
@@ -3363,14 +3653,14 @@
       <c r="R31" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="T31" s="2" t="s">
+      <c r="S31" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="U31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>150</v>
       </c>
@@ -3378,7 +3668,7 @@
         <v>151</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>140</v>
@@ -3419,22 +3709,22 @@
       <c r="R32" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="T32" s="2" t="s">
+      <c r="S32" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="U32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>176</v>
       </c>
       <c r="B33" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>2</v>
@@ -3475,22 +3765,22 @@
       <c r="R33" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="T33" s="2" t="s">
+      <c r="S33" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="U33" t="s">
+      <c r="T33" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>177</v>
       </c>
       <c r="B34" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>2</v>
@@ -3531,22 +3821,22 @@
       <c r="R34" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="T34" s="2" t="s">
+      <c r="S34" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="U34" t="s">
+      <c r="T34" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>178</v>
       </c>
       <c r="B35" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>2</v>
@@ -3587,22 +3877,22 @@
       <c r="R35" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="T35" s="2" t="s">
+      <c r="S35" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="U35" t="s">
+      <c r="T35" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>179</v>
       </c>
       <c r="B36" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>2</v>
@@ -3643,37 +3933,37 @@
       <c r="R36" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="T36" s="2" t="s">
+      <c r="S36" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="U36" t="s">
+      <c r="T36" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>198</v>
+      </c>
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" t="s">
+        <v>350</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B37" t="s">
-        <v>195</v>
-      </c>
-      <c r="C37" t="s">
-        <v>351</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I37" s="2">
         <v>300</v>
@@ -3688,51 +3978,51 @@
         <v>2017</v>
       </c>
       <c r="M37" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="N37" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="N37" s="5" t="s">
-        <v>356</v>
-      </c>
       <c r="P37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q37" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R37" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="S37" s="2" t="s">
         <v>205</v>
       </c>
       <c r="T37" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>206</v>
       </c>
-      <c r="U37" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>207</v>
-      </c>
       <c r="B38" t="s">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I38" s="2">
         <v>1000</v>
@@ -3747,48 +4037,48 @@
         <v>2022</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q38" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R38" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="S38" s="2" t="s">
         <v>213</v>
       </c>
       <c r="T38" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>214</v>
       </c>
-      <c r="U38" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>215</v>
-      </c>
       <c r="B39" t="s">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I39" s="2">
         <v>100</v>
@@ -3803,33 +4093,33 @@
         <v>2018</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q39" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R39" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="S39" s="2" t="s">
         <v>216</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="U39" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B40" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>35</v>
@@ -3844,7 +4134,7 @@
         <v>35</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>26</v>
@@ -3859,48 +4149,48 @@
         <v>2017</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q40" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R40" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T40" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>225</v>
       </c>
-      <c r="T40" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="U40" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
+        <v>230</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B41" t="s">
-        <v>231</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="E41" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>26</v>
@@ -3915,48 +4205,48 @@
         <v>2023</v>
       </c>
       <c r="M41" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="N41" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="N41" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="Q41" s="2" t="b">
         <v>0</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="T41" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="U41" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B42" t="s">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I42" s="2">
         <v>8500</v>
@@ -3971,51 +4261,51 @@
         <v>2010</v>
       </c>
       <c r="M42" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="N42" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="N42" s="2" t="s">
+      <c r="O42" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="O42" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="Q42" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R42" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="S42" s="2" t="s">
         <v>255</v>
       </c>
       <c r="T42" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="U42" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B43" t="s">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I43" s="2">
         <v>8500</v>
@@ -4030,51 +4320,51 @@
         <v>2010</v>
       </c>
       <c r="M43" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="N43" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="N43" s="2" t="s">
+      <c r="O43" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="O43" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="Q43" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R43" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="S43" s="2" t="s">
         <v>255</v>
       </c>
       <c r="T43" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="U43" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B44" t="s">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I44" s="2">
         <v>8500</v>
@@ -4089,51 +4379,51 @@
         <v>2010</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N44" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="O44" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="O44" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="Q44" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="S44" s="2" t="s">
+        <v>256</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="U44" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B45" t="s">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I45" s="2">
         <v>8500</v>
@@ -4148,51 +4438,51 @@
         <v>2010</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N45" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="O45" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="O45" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="Q45" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>256</v>
       </c>
       <c r="T45" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="U45" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B46" t="s">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I46" s="2">
         <v>8500</v>
@@ -4207,51 +4497,51 @@
         <v>2010</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N46" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="O46" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="O46" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="Q46" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>257</v>
       </c>
       <c r="T46" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="U46" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" ht="15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B47" t="s">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I47" s="2">
         <v>8500</v>
@@ -4266,42 +4556,42 @@
         <v>2010</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N47" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="O47" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="O47" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="Q47" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="S47" s="2" t="s">
+        <v>257</v>
       </c>
       <c r="T47" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="U47" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B48" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>9</v>
@@ -4310,7 +4600,7 @@
         <v>80</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I48" s="2">
         <v>1000</v>
@@ -4325,13 +4615,13 @@
         <v>2019</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N48" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="O48" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="O48" s="2" t="s">
-        <v>268</v>
       </c>
       <c r="Q48" s="2" t="b">
         <v>1</v>
@@ -4339,37 +4629,37 @@
       <c r="R48" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="S48" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="T48" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="U48" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>268</v>
+      </c>
+      <c r="B49" t="s">
         <v>269</v>
       </c>
-      <c r="B49" t="s">
-        <v>270</v>
-      </c>
       <c r="C49" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I49" s="2">
         <v>500</v>
@@ -4384,42 +4674,42 @@
         <v>2023</v>
       </c>
       <c r="M49" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="N49" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="N49" s="2" t="s">
+      <c r="O49" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="O49" s="2" t="s">
-        <v>274</v>
       </c>
       <c r="Q49" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R49" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="S49" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="T49" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="U49" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T49" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B50" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>9</v>
@@ -4428,7 +4718,7 @@
         <v>2</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I50" s="2">
         <v>11000</v>
@@ -4443,42 +4733,42 @@
         <v>2023</v>
       </c>
       <c r="M50" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="N50" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="N50" s="2" t="s">
+      <c r="O50" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="O50" s="2" t="s">
-        <v>289</v>
       </c>
       <c r="Q50" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R50" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="S50" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="T50" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="T50" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="U50" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B51" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>9</v>
@@ -4487,7 +4777,7 @@
         <v>2</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I51" s="2">
         <v>11000</v>
@@ -4502,39 +4792,39 @@
         <v>2023</v>
       </c>
       <c r="M51" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="N51" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="N51" s="2" t="s">
-        <v>288</v>
       </c>
       <c r="Q51" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R51" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="S51" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="T51" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="T51" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="U51" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B52" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>9</v>
@@ -4543,7 +4833,7 @@
         <v>2</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I52" s="2">
         <v>11000</v>
@@ -4558,42 +4848,42 @@
         <v>2023</v>
       </c>
       <c r="M52" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="N52" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="N52" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="P52" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="Q52" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R52" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
+      </c>
+      <c r="S52" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="T52" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="U52" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>282</v>
+      </c>
+      <c r="B53" t="s">
         <v>283</v>
       </c>
-      <c r="B53" t="s">
-        <v>284</v>
-      </c>
       <c r="C53" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>9</v>
@@ -4602,7 +4892,7 @@
         <v>2</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I53" s="2">
         <v>11000</v>
@@ -4617,42 +4907,42 @@
         <v>2023</v>
       </c>
       <c r="M53" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="N53" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="N53" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="P53" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="Q53" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R53" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
+      </c>
+      <c r="S53" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="T53" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="U53" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>297</v>
+      </c>
+      <c r="B54" t="s">
         <v>298</v>
       </c>
-      <c r="B54" t="s">
-        <v>299</v>
-      </c>
       <c r="C54" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>36</v>
@@ -4676,48 +4966,48 @@
         <v>2023</v>
       </c>
       <c r="M54" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="N54" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="N54" s="2" t="s">
-        <v>302</v>
       </c>
       <c r="Q54" s="2" t="b">
         <v>0</v>
       </c>
       <c r="R54" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="S54" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T54" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>304</v>
       </c>
-      <c r="U54" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>305</v>
-      </c>
       <c r="B55" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>311</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I55" s="2">
         <v>30</v>
@@ -4732,54 +5022,54 @@
         <v>2022</v>
       </c>
       <c r="M55" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="N55" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O55" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="N55" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="O55" s="2" t="s">
-        <v>324</v>
-      </c>
       <c r="P55" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q55" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R55" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="S55" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="T55" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="U55" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B56" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I56" s="2">
         <v>30</v>
@@ -4794,54 +5084,54 @@
         <v>2022</v>
       </c>
       <c r="M56" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="N56" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O56" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="N56" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="O56" s="2" t="s">
-        <v>324</v>
-      </c>
       <c r="P56" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Q56" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="T56" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="U56" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="S56" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="T56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B57" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I57" s="2">
         <v>30</v>
@@ -4856,54 +5146,54 @@
         <v>2022</v>
       </c>
       <c r="M57" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="N57" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O57" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="N57" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="O57" s="2" t="s">
-        <v>324</v>
-      </c>
       <c r="P57" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q57" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R57" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="T57" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="U57" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="S57" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="T57" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B58" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I58" s="2">
         <v>30</v>
@@ -4918,54 +5208,54 @@
         <v>2022</v>
       </c>
       <c r="M58" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="N58" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O58" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="N58" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="O58" s="2" t="s">
-        <v>324</v>
-      </c>
       <c r="P58" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q58" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R58" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="T58" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="U58" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="S58" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="T58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>308</v>
+      </c>
+      <c r="B59" t="s">
+        <v>320</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B59" t="s">
-        <v>321</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>310</v>
-      </c>
       <c r="E59" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I59" s="2">
         <v>30</v>
@@ -4980,34 +5270,34 @@
         <v>2022</v>
       </c>
       <c r="M59" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="N59" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="O59" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="N59" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="O59" s="2" t="s">
-        <v>324</v>
-      </c>
       <c r="P59" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q59" s="2" t="b">
         <v>1</v>
       </c>
       <c r="R59" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="T59" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="S59" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="T59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>331</v>
       </c>
-      <c r="U59" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>332</v>
-      </c>
       <c r="B60" t="s">
         <v>26</v>
       </c>
@@ -5015,16 +5305,16 @@
         <v>26</v>
       </c>
       <c r="D60" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>335</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>336</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>25</v>
@@ -5051,18 +5341,18 @@
         <v>0</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="T60" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="U60" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+      <c r="S60" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="T60" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B61" t="s">
         <v>26</v>
@@ -5071,16 +5361,16 @@
         <v>26</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>25</v>
@@ -5107,36 +5397,36 @@
         <v>0</v>
       </c>
       <c r="R61" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="T61" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="U61" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+      <c r="S61" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="T61" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>333</v>
+      </c>
+      <c r="B62" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B62" t="s">
-        <v>26</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>335</v>
-      </c>
       <c r="E62" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>25</v>
@@ -5163,19 +5453,612 @@
         <v>0</v>
       </c>
       <c r="R62" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="T62" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="U62" t="s">
+        <v>302</v>
+      </c>
+      <c r="S62" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="T62" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>366</v>
+      </c>
+      <c r="B63" t="s">
+        <v>367</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="I63" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K63" s="2">
+        <v>2019</v>
+      </c>
+      <c r="L63" s="2">
+        <v>2021</v>
+      </c>
+      <c r="M63" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="N63" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="O63" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="P63" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q63" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R63" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="S63" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="T63" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>369</v>
+      </c>
+      <c r="B64" t="s">
+        <v>370</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="I64" s="2">
+        <v>25</v>
+      </c>
+      <c r="J64" s="2">
+        <v>30</v>
+      </c>
+      <c r="K64" s="2">
+        <v>2019</v>
+      </c>
+      <c r="L64" s="2">
+        <v>2022</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="N64" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="O64" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q64" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R64" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="S64" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="T64" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>378</v>
+      </c>
+      <c r="B65" t="s">
+        <v>370</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="I65" s="2">
+        <v>25</v>
+      </c>
+      <c r="J65" s="2">
+        <v>30</v>
+      </c>
+      <c r="K65" s="2">
+        <v>2019</v>
+      </c>
+      <c r="L65" s="2">
+        <v>2022</v>
+      </c>
+      <c r="M65" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="N65" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="O65" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q65" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R65" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="S65" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="T65" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>379</v>
+      </c>
+      <c r="B66" t="s">
+        <v>370</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="I66" s="2">
+        <v>25</v>
+      </c>
+      <c r="J66" s="2">
+        <v>30</v>
+      </c>
+      <c r="K66" s="2">
+        <v>2019</v>
+      </c>
+      <c r="L66" s="2">
+        <v>2022</v>
+      </c>
+      <c r="M66" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="N66" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="O66" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q66" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R66" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="S66" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="T66" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>380</v>
+      </c>
+      <c r="B67" t="s">
+        <v>370</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="I67" s="2">
+        <v>25</v>
+      </c>
+      <c r="J67" s="2">
+        <v>30</v>
+      </c>
+      <c r="K67" s="2">
+        <v>2019</v>
+      </c>
+      <c r="L67" s="2">
+        <v>2022</v>
+      </c>
+      <c r="M67" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="N67" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="O67" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q67" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R67" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="S67" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="T67" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>397</v>
+      </c>
+      <c r="B68" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="I68" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K68" s="2">
+        <v>2019</v>
+      </c>
+      <c r="L68" s="2">
+        <v>2022</v>
+      </c>
+      <c r="M68" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="N68" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q68" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R68" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="S68" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="T68" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>402</v>
+      </c>
+      <c r="B69" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="I69" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K69" s="2">
+        <v>1970</v>
+      </c>
+      <c r="L69" s="2">
+        <v>2000</v>
+      </c>
+      <c r="M69" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="N69" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="O69" t="s">
+        <v>409</v>
+      </c>
+      <c r="P69" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q69" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R69" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="S69" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="T69" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>413</v>
+      </c>
+      <c r="B70" t="s">
+        <v>414</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="I70" s="2">
+        <v>30</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K70" s="2">
+        <v>2000</v>
+      </c>
+      <c r="L70" s="2">
+        <v>2022</v>
+      </c>
+      <c r="M70" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="N70" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="O70" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="P70" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q70" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R70" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="S70" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="T70" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>424</v>
+      </c>
+      <c r="B71" t="s">
+        <v>425</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="I71" s="2">
+        <v>250</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K71" s="2">
+        <v>2000</v>
+      </c>
+      <c r="L71" s="2">
+        <v>2022</v>
+      </c>
+      <c r="M71" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="N71" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="O71" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="P71" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q71" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R71" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="S71" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="T71" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>434</v>
+      </c>
+      <c r="B72" t="s">
+        <v>26</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K72" s="2">
+        <v>2000</v>
+      </c>
+      <c r="L72" s="2">
+        <v>2022</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="N72" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="O72" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="Q72" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R72" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="S72" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="T72" s="2" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576 C22 C37:C39" xr:uid="{B8A4A375-095B-4B65-8BFA-EF4550E341DF}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22 C37:C39 A1:A1048576" xr:uid="{B8A4A375-095B-4B65-8BFA-EF4550E341DF}">
       <formula1>COUNTIF(A:A,A1)&lt;2</formula1>
     </dataValidation>
   </dataValidations>
@@ -5191,8 +6074,12 @@
     <hyperlink ref="N56:N59" r:id="rId9" display="https://onlinelibrary.wiley.com/doi/abs/10.1111/geb.12365" xr:uid="{2168C62F-3D18-4D95-A345-3FF3E957168C}"/>
     <hyperlink ref="M22" r:id="rId10" xr:uid="{D8977355-2E06-472C-861E-C2C127DA83B3}"/>
     <hyperlink ref="N37" r:id="rId11" xr:uid="{F73861C8-5C17-479D-83F0-158B7B267EC8}"/>
+    <hyperlink ref="O63" r:id="rId12" display="https://doi.org/10.3334/ORNLDAAC/2017" xr:uid="{4AFDE2B0-4FD0-4F0F-8979-FB0C9ECA875A}"/>
+    <hyperlink ref="N65" r:id="rId13" xr:uid="{E71FBFBA-3A68-4EB2-BE1A-892D9C15339A}"/>
+    <hyperlink ref="N66" r:id="rId14" xr:uid="{F92CDA0C-CEB4-4D56-898C-CA812401C055}"/>
+    <hyperlink ref="N67" r:id="rId15" xr:uid="{5AD05759-E8D5-4CDD-831B-BCB1F576DDC3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>